<commit_message>
Docs: Add instructions for running tests and generating coverage report
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCases_Login_Register.xlsx
+++ b/src/main/resources/TestCases_Login_Register.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -79,18 +79,6 @@
     <t>User is redirected to Forgot Password page</t>
   </si>
   <si>
-    <t>L05</t>
-  </si>
-  <si>
-    <t>Verify 'Remember Me' functionality</t>
-  </si>
-  <si>
-    <t>Enter credentials, check 'Remember Me', login and logout</t>
-  </si>
-  <si>
-    <t>User credentials remain saved on next visit</t>
-  </si>
-  <si>
     <t>R01</t>
   </si>
   <si>
@@ -128,18 +116,6 @@
   </si>
   <si>
     <t>R04</t>
-  </si>
-  <si>
-    <t>Verify password strength validation</t>
-  </si>
-  <si>
-    <t>Enter weak password in registration form</t>
-  </si>
-  <si>
-    <t>Error message displayed for weak password</t>
-  </si>
-  <si>
-    <t>R05</t>
   </si>
   <si>
     <t>Verify confirm password validation</t>
@@ -254,7 +230,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -271,9 +247,6 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1356,7 +1329,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1364,9 +1337,9 @@
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5234" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.2109" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.0859" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6484" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.3359" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7969" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1387,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="26.55" customHeight="1">
+    <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>5</v>
       </c>
@@ -1438,7 +1411,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" ht="31.75" customHeight="1">
       <c r="A5" t="s" s="5">
         <v>18</v>
       </c>
@@ -1455,29 +1428,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" ht="35.6" customHeight="1">
       <c r="A6" t="s" s="5">
         <v>22</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" ht="40.5" customHeight="1">
+      <c r="A7" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s" s="5">
         <v>23</v>
-      </c>
-      <c r="D6" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>27</v>
       </c>
       <c r="C7" t="s" s="5">
         <v>28</v>
@@ -1489,12 +1462,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" ht="44.3" customHeight="1">
       <c r="A8" t="s" s="5">
         <v>31</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s" s="5">
         <v>32</v>
@@ -1503,66 +1476,25 @@
         <v>33</v>
       </c>
       <c r="E8" t="s" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" ht="62" customHeight="1">
+      <c r="A9" t="s" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="5">
+      <c r="B9" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="5">
         <v>35</v>
       </c>
-      <c r="B9" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s" s="5">
+      <c r="D9" t="s" s="5">
         <v>36</v>
       </c>
-      <c r="D9" t="s" s="5">
+      <c r="E9" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="E9" t="s" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s" s="5">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s" s="5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="5">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>